<commit_message>
fazer o cruzamento das planilhas e calcular a remuneração
</commit_message>
<xml_diff>
--- a/output/termo complementar.xlsx
+++ b/output/termo complementar.xlsx
@@ -463,7 +463,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>C000000825018</t>
+          <t>C825018</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -485,7 +485,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>C000000825020</t>
+          <t>C825020</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -507,7 +507,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>C000000825021</t>
+          <t>C825021</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -529,7 +529,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>C000000825019</t>
+          <t>C825019</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -551,7 +551,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>C000000825020</t>
+          <t>C825020</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">

</xml_diff>